<commit_message>
adding more docs and training data
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trentconley/Desktop/Work/Discord-Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148245B6-20F4-084A-8740-528B78986077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2893105-B6E0-6C44-91B3-7E40E4137165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{EAE3276D-B296-5145-A0E6-066B62DA037C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Message</t>
   </si>
@@ -129,13 +129,64 @@
   </si>
   <si>
     <t>Please paste your transaction id and wallet id below</t>
+  </si>
+  <si>
+    <t>I saw messege in chat, I have completed testnet of 5 days but no role no nft received.</t>
+  </si>
+  <si>
+    <t>Have you change your discord name since you've completed the testnet tasks? What is the full ETH address?</t>
+  </si>
+  <si>
+    <t>the query is I have completed that five days task. but didn't get nft or role</t>
+  </si>
+  <si>
+    <t>Please provide screenshots showing that you completed the steps. Also, make sure you have minted the NFT. NFT drops whitelist your address, but do not automatically deposit it.</t>
+  </si>
+  <si>
+    <t>i can't claim my pioneer nft but i have claimed. my address 0x7fB87Ff912b81A9211fb4cca2445643702bf5D33</t>
+  </si>
+  <si>
+    <t>Could you please clarify ... You can't claim but have claimed?</t>
+  </si>
+  <si>
+    <t>i can't claim role hahah. and i can't mint them. so that's why am not eligble</t>
+  </si>
+  <si>
+    <t>Without a tx id it's hard to know why these are failing, could you please provide that?</t>
+  </si>
+  <si>
+    <t>Dont get points. 0xBb41dd49254E8B9d631B835062392a460081734D.</t>
+  </si>
+  <si>
+    <t>Hello. If you have deposited recently, please refresh and check again later. More info regarding points can be found here. https://docs.primeprotocol.xyz/navigating-prime/prime-early-adopter-program</t>
+  </si>
+  <si>
+    <t>Hello. I noticed that when you repay the loan and withdraw the deposit, if you use the button 100%, then the entire amount is not withdrawn, the account balance is left, which will have to repay again and of course pay for gas.</t>
+  </si>
+  <si>
+    <t>Thank you for the information; I'll tag the team on this.</t>
+  </si>
+  <si>
+    <t>0x9E3CeB09375f9d4922D6dc7Da3D006958298CDA8, id like to re-add my initial deposit - which was much more. really like how the P P team handled all this. im sure though you can understand my concerns about liquidity and rewards - i think you all will do great. lmk about the points</t>
+  </si>
+  <si>
+    <t>i deposit some glmr and dot, but I can't withdraw it. I found some errors in the execution of the contract, please help me to see if I can get my token back. my tx: 0xb6d674171cf570185a5ad3ddef47f853b71d4e923d139d0739d03c0bdc2fa319 0x0d54faeba552e9f5f0f4ad322800ed6f6539e4c4e74348171b09bfecb899831b</t>
+  </si>
+  <si>
+    <t>Thank you for providing the transaction. I have tagged the team and they will continue from here.</t>
+  </si>
+  <si>
+    <t>If I didn't get the daily connect posted yesterday before the zealy renewal time, doesn't this sprint count? After all, I'm shorted by 50xp for one daily connect, right?</t>
+  </si>
+  <si>
+    <t>If you can't complete this task. You won't get XP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,30 +197,6 @@
     <font>
       <sz val="16"/>
       <color rgb="FFDCDDDE"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11.4"/>
-      <color rgb="FFDCDDDE"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="17"/>
-      <color rgb="FF0096CF"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -194,14 +221,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,7 +255,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -570,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0F653C-8C28-2E41-92CF-BB2F31002CAC}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,8 +677,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>2022</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -665,64 +688,150 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2034</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2038</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2109</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1975</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
+      <c r="A11" s="2">
+        <v>1955</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>1954</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>1948</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>1910</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>1933</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>1942</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>1986</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>1925</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>